<commit_message>
Data preparation 50% ready, read_data finished
</commit_message>
<xml_diff>
--- a/data_preparation/inputs_folder_name/Allocation Matrix.xlsx
+++ b/data_preparation/inputs_folder_name/Allocation Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\OneDrive\Escritorio\2023\Forecasting\dta\data_preparation\inputs_folder_name\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D35F72CC-9085-411B-B7E8-4E316C1F5FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D432F4-B8AD-4FE8-AE1C-4251B3367BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dimensions Name" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>SKU from</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t>Desc</t>
+  </si>
+  <si>
+    <t>skuf</t>
+  </si>
+  <si>
+    <t>skut</t>
   </si>
 </sst>
 </file>
@@ -550,7 +556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77757BD9-4B68-4578-AC39-0BFD007C3FCF}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -640,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C734"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -664,9 +670,15 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>

</xml_diff>